<commit_message>
rerunning all figures. Resetting one NMDS with soil variables only.
</commit_message>
<xml_diff>
--- a/R/nutrient_summary.xlsx
+++ b/R/nutrient_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martef\DokumenterIntern\GitHub\GRAN_revegetation_new\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB021BC-4497-4D57-9599-2B6C08BAA264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB614A6C-FDAC-43C8-8FAA-D6E6E7CF6D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12600" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12600" yWindow="-18120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treatment" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="256">
   <si>
     <t>Treatment</t>
   </si>
@@ -1268,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1615,11 +1615,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -1819,6 +1834,94 @@
       </c>
       <c r="P4" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" t="s">
+        <v>231</v>
+      </c>
+      <c r="D6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>229</v>
+      </c>
+      <c r="G6" t="s">
+        <v>227</v>
+      </c>
+      <c r="H6" t="s">
+        <v>225</v>
+      </c>
+      <c r="I6" t="s">
+        <v>224</v>
+      </c>
+      <c r="J6" t="s">
+        <v>228</v>
+      </c>
+      <c r="K6" t="s">
+        <v>222</v>
+      </c>
+      <c r="L6" t="s">
+        <v>221</v>
+      </c>
+      <c r="M6" t="s">
+        <v>226</v>
+      </c>
+      <c r="N6" t="s">
+        <v>233</v>
+      </c>
+      <c r="O6" t="s">
+        <v>232</v>
+      </c>
+      <c r="P6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>255</v>
+      </c>
+      <c r="D7" t="s">
+        <v>239</v>
+      </c>
+      <c r="F7" t="s">
+        <v>246</v>
+      </c>
+      <c r="G7" t="s">
+        <v>243</v>
+      </c>
+      <c r="H7" t="s">
+        <v>237</v>
+      </c>
+      <c r="I7" t="s">
+        <v>240</v>
+      </c>
+      <c r="J7" t="s">
+        <v>245</v>
+      </c>
+      <c r="K7" t="s">
+        <v>235</v>
+      </c>
+      <c r="L7" t="s">
+        <v>254</v>
+      </c>
+      <c r="M7" t="s">
+        <v>236</v>
+      </c>
+      <c r="O7" t="s">
+        <v>238</v>
+      </c>
+      <c r="P7" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>